<commit_message>
Fixed Fat from sliding
</commit_message>
<xml_diff>
--- a/doc/mslug5-addresses.xlsx
+++ b/doc/mslug5-addresses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Emulators\MAME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Romhack Projects\Metal Slug 5 - No Slide\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201C0142-1337-43F0-8025-105669F78F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F39C55-3612-46B2-A51E-3A57AD4A44FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13380" yWindow="8805" windowWidth="13725" windowHeight="10980" xr2:uid="{C1C3456E-20F6-4FC4-BD16-94C28D891507}"/>
+    <workbookView xWindow="-13515" yWindow="7155" windowWidth="13380" windowHeight="14145" xr2:uid="{C1C3456E-20F6-4FC4-BD16-94C28D891507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="154">
   <si>
     <t>Certain Animation Frame Counter</t>
   </si>
@@ -395,9 +395,6 @@
     <t>01F4D2</t>
   </si>
   <si>
-    <t>WORKED !!@@!@!!@@ changed BNE &gt; BEQ skips crawling slide</t>
-  </si>
-  <si>
     <t>070054</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t>01F6F6</t>
   </si>
   <si>
-    <t>WORKED @@!!@!@!@ changed from BNE &gt; BEQ aka 66 to 67 shooting while sliding</t>
-  </si>
-  <si>
     <t>01EC1A</t>
   </si>
   <si>
@@ -468,6 +462,42 @@
   </si>
   <si>
     <t>66 &gt; 67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skips crawling slide but makes crawling slide when FAT </t>
+  </si>
+  <si>
+    <t>01F6FE</t>
+  </si>
+  <si>
+    <t>66 &gt; 67 later test to skip when fat or skinny</t>
+  </si>
+  <si>
+    <t>01EDD4</t>
+  </si>
+  <si>
+    <t>01ECDC</t>
+  </si>
+  <si>
+    <t>01EF5A</t>
+  </si>
+  <si>
+    <t>01F392</t>
+  </si>
+  <si>
+    <t>01F58E</t>
+  </si>
+  <si>
+    <t>66 &gt; 60</t>
+  </si>
+  <si>
+    <t>happens when fat.</t>
+  </si>
+  <si>
+    <t>NOP NOP 71 4E 71 4E</t>
+  </si>
+  <si>
+    <t>NOP NOP</t>
   </si>
 </sst>
 </file>
@@ -553,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -570,6 +600,7 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,16 +935,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9662A68B-5007-4C0B-9772-142E984CDAA6}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B68" sqref="B67:B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -993,7 +1024,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -1371,7 +1402,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
         <v>104</v>
@@ -1387,7 +1418,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
         <v>107</v>
@@ -1406,12 +1437,12 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1427,10 +1458,10 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,128 +1493,253 @@
         <v>118</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>128</v>
+      <c r="B75" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B77" s="6" t="s">
+      <c r="A77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="B79" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B90" s="6" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="16"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="16"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>143</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="str">
+        <f t="shared" ref="B108:B110" si="0">UPPER(A108)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>